<commit_message>
Updates Registo Horas Form and adds new form for registering documents
</commit_message>
<xml_diff>
--- a/X_LEGEND_registo_horas/LEGEND_X_registo_horas-media/LEGEND_X_registo_horas.xlsx
+++ b/X_LEGEND_registo_horas/LEGEND_X_registo_horas-media/LEGEND_X_registo_horas.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\legend\ODK Forms\Forms in current use\X_LEGEND_registo_horas\LEGEND_registo_horas-media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\legend\ODK Forms\legend-odk-forms\X_LEGEND_registo_horas\LEGEND_X_registo_horas-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9795" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9795" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">choices!$A$1:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="119">
   <si>
     <t>type</t>
   </si>
@@ -345,22 +345,65 @@
     <t>LEGEND X Registo Horas</t>
   </si>
   <si>
-    <t>Sensibilização, formação de associações, actividades de delimitação</t>
-  </si>
-  <si>
     <t>Completou qualquer formulário do processo?</t>
   </si>
   <si>
     <t>Quantos formulários foram completados?</t>
+  </si>
+  <si>
+    <t>Sensibilização</t>
+  </si>
+  <si>
+    <t>Actividades de associativismo</t>
+  </si>
+  <si>
+    <t>Plano de Uso de Terra</t>
+  </si>
+  <si>
+    <t>Identificação de limites de povoados</t>
+  </si>
+  <si>
+    <t>Actividades de DRP (delimitação comunitária)</t>
+  </si>
+  <si>
+    <t>Objecções e Correções</t>
+  </si>
+  <si>
+    <t>Actividades de georeferenciamento e/ou devolução</t>
+  </si>
+  <si>
+    <t>obj_corr</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>geo_dev</t>
+  </si>
+  <si>
+    <t>drp</t>
+  </si>
+  <si>
+    <t>limites_pov</t>
+  </si>
+  <si>
+    <t>assoc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -550,339 +593,342 @@
   </borders>
   <cellStyleXfs count="236">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="236">
@@ -1119,9 +1165,9 @@
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="233"/>
-    <cellStyle name="Normal 3" xfId="234"/>
-    <cellStyle name="Normal 3 2" xfId="235"/>
+    <cellStyle name="Normal 2" xfId="233" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="Normal 3" xfId="234" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="Normal 3 2" xfId="235" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1457,14 +1503,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,7 +1626,7 @@
       <c r="B5" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="49" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1675,8 +1721,8 @@
       <c r="B11" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>105</v>
+      <c r="C11" s="48" t="s">
+        <v>104</v>
       </c>
       <c r="J11" s="30" t="s">
         <v>22</v>
@@ -1692,8 +1738,8 @@
       <c r="B12" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="49" t="s">
-        <v>106</v>
+      <c r="C12" s="48" t="s">
+        <v>105</v>
       </c>
       <c r="G12" s="43" t="s">
         <v>77</v>
@@ -1761,14 +1807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,56 +2043,122 @@
       <c r="B20" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="48" t="s">
-        <v>104</v>
+      <c r="C20" s="50" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>53</v>
+      <c r="B21" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="28" t="s">
-        <v>54</v>
+      <c r="B22" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>55</v>
+      <c r="B23" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="51" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="50" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C30" s="28" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D13"/>
+  <autoFilter ref="A1:D13" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <sortState ref="C14:C18">
     <sortCondition ref="C14:C18"/>
   </sortState>
@@ -2056,11 +2168,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,7 +2206,7 @@
         <v>78</v>
       </c>
       <c r="C2" s="5">
-        <v>201707081</v>
+        <v>201710181</v>
       </c>
       <c r="D2" s="35" t="s">
         <v>68</v>

</xml_diff>